<commit_message>
Mise a jour de la documentation et débout d'un petit code sur CLion
Dans ce commit, j'ai un peu commencé le code, mais avec beaucoup d'échecs.
J'ai voulu faire un menu pour le débout.

La documentation, j'ai mis a jour le journal de travail, commencé le MCD pourtant je crois qu'il me manque encore des tables.
</commit_message>
<xml_diff>
--- a/Documentation/Use Case Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Use Case Bataille Navale Rui_Monteiro.xlsx
@@ -5,24 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rui-Miguel.MONTEIRO\Google Drive\CPNV\1ére année\Modules\ICT\431\Bataille Navale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.Modules\MA\20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="8" r:id="rId1"/>
-    <sheet name="Use case" sheetId="3" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
-    <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil5" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil6" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil7" sheetId="7" r:id="rId7"/>
-    <sheet name="Parametres" sheetId="2" r:id="rId8"/>
+    <sheet name="Use case scénario" sheetId="3" r:id="rId2"/>
+    <sheet name="User case lancer un programme" sheetId="1" r:id="rId3"/>
+    <sheet name="User case mettre l'identifiant" sheetId="4" r:id="rId4"/>
+    <sheet name="User case lancer une partie" sheetId="5" r:id="rId5"/>
+    <sheet name="User case jouer" sheetId="6" r:id="rId6"/>
+    <sheet name="Parametres" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t>Identifiant + Titre</t>
   </si>
@@ -72,12 +70,33 @@
   <si>
     <t>Utilisateur</t>
   </si>
+  <si>
+    <t>Lancer le programme</t>
+  </si>
+  <si>
+    <t>Lancer une partie</t>
+  </si>
+  <si>
+    <t>Jouer</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Mettre l'dentifiant</t>
+  </si>
+  <si>
+    <t>BN_Lancement du programme</t>
+  </si>
+  <si>
+    <t>Jouer à la bataille navale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +104,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -395,6 +428,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,32 +473,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,6 +500,331 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Émoticône 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="571500"/>
+          <a:ext cx="761999" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="smileyFace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Flèche droite 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="1343025"/>
+          <a:ext cx="1104900" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Flèche droite 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1171575" y="1714500"/>
+          <a:ext cx="1104900" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Flèche droite 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1171575" y="2095500"/>
+          <a:ext cx="1104900" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Flèche droite 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1171575" y="2476500"/>
+          <a:ext cx="1104900" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085850" y="1152525"/>
+          <a:ext cx="95250" cy="1504950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -725,8 +1095,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,15 +1110,63 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D14:F14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -760,7 +1178,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -770,104 +1188,126 @@
   <sheetData>
     <row r="1" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="15"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
@@ -881,28 +1321,22 @@
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D6:G6"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D6:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Parametres!$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:G3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -918,7 +1352,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -928,50 +1362,52 @@
   <sheetData>
     <row r="1" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -979,59 +1415,65 @@
     </row>
     <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="B6:C6"/>
@@ -1039,28 +1481,28 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D6:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Parametres!$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:G3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1076,7 +1518,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1086,50 +1528,52 @@
   <sheetData>
     <row r="1" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -1137,59 +1581,65 @@
     </row>
     <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="B6:C6"/>
@@ -1197,28 +1647,28 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D6:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Parametres!$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:G3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1234,7 +1684,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1244,50 +1694,52 @@
   <sheetData>
     <row r="1" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -1295,59 +1747,65 @@
     </row>
     <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="B6:C6"/>
@@ -1355,28 +1813,28 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D6:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Parametres!$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:G3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1387,170 +1845,12 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="B1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="11.85546875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Parametres!$B$3:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D6:G6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.42578125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>